<commit_message>
Added IMCS parameter matrix
</commit_message>
<xml_diff>
--- a/Kirby/Excel Files/RESOURCE_USAGE_PARAMETERS.xlsx
+++ b/Kirby/Excel Files/RESOURCE_USAGE_PARAMETERS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirbsand.AUTH\Documents\GitHub\Group-13-HP-Big-Data-Analytics\Kirby\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nic\Projects\Group-13-HP-Big-Data-Analytics\Kirby\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Experiment 1" sheetId="3" r:id="rId2"/>
     <sheet name="Memory Allocation" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
   <si>
     <t>PGA_AGGREGATE_LIMIT</t>
   </si>
@@ -203,12 +203,39 @@
   </si>
   <si>
     <t>DB_BIG_TABLE_CACHE_TARGET_PERCENT</t>
+  </si>
+  <si>
+    <t>Experiment # X</t>
+  </si>
+  <si>
+    <t>NO MEMCOMPRESS</t>
+  </si>
+  <si>
+    <t>MEMCOMPRESS FOR DML</t>
+  </si>
+  <si>
+    <t>MEMCOMPRESS FOR QUERY LOW</t>
+  </si>
+  <si>
+    <t>IMCS Compression</t>
+  </si>
+  <si>
+    <t>0G</t>
+  </si>
+  <si>
+    <t>MEMCOMPRESS FOR QUERY HIGH</t>
+  </si>
+  <si>
+    <t>MEMCOMPRESS FOR CAPACITY LOW</t>
+  </si>
+  <si>
+    <t>MEMCOMPRESS FOR CAPACITY HIGH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -562,7 +589,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -682,6 +709,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D6D8-432F-994D-8EAF1D0A948F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -702,6 +734,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-D6D8-432F-994D-8EAF1D0A948F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -722,6 +759,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-D6D8-432F-994D-8EAF1D0A948F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -742,6 +784,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-D6D8-432F-994D-8EAF1D0A948F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -784,6 +831,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-D6D8-432F-994D-8EAF1D0A948F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1541,6 +1593,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1576,6 +1645,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1734,14 +1820,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="26" t="s">
         <v>46</v>
       </c>
@@ -1750,7 +1836,7 @@
       <c r="D1" s="27"/>
       <c r="E1" s="28"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1767,7 +1853,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1784,7 +1870,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1801,7 +1887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1818,7 +1904,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1835,7 +1921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1852,7 +1938,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1869,7 +1955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1903,15 +1989,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="1:5" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A12" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="31"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1922,7 +2008,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1933,7 +2019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1944,7 +2030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1955,7 +2041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1966,7 +2052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -1977,7 +2063,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1988,7 +2074,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
@@ -1999,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -2010,7 +2096,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -2021,7 +2107,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -2032,7 +2118,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
@@ -2043,15 +2129,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="26" spans="1:3" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A26" s="29" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="31"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2060,7 +2146,7 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -2069,7 +2155,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
@@ -2103,20 +2189,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="20.5703125" customWidth="1"/>
-    <col min="5" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20.59765625" customWidth="1"/>
+    <col min="5" max="6" width="25.73046875" customWidth="1"/>
+    <col min="7" max="7" width="48.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="33.75" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A1" s="32" t="s">
         <v>54</v>
       </c>
@@ -2128,7 +2214,7 @@
       <c r="F1" s="33"/>
       <c r="G1" s="34"/>
     </row>
-    <row r="2" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="20" t="s">
         <v>55</v>
       </c>
@@ -2148,7 +2234,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -2168,7 +2254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2188,7 +2274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -2208,7 +2294,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -2228,7 +2314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2248,7 +2334,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -2268,7 +2354,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A9" s="23">
         <v>7</v>
       </c>
@@ -2288,7 +2374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2308,7 +2394,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -2328,11 +2414,97 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:7" ht="33.75" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="E13" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E14" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="E15" s="23">
+        <v>1</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E17" s="7">
+        <v>3</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="E18" s="23">
+        <v>4</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E19" s="3">
+        <v>5</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E20" s="7">
+        <v>6</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2347,13 +2519,13 @@
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -2361,7 +2533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2369,7 +2541,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2377,7 +2549,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2385,7 +2557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>33</v>
       </c>

</xml_diff>